<commit_message>
big dump, clean up later
</commit_message>
<xml_diff>
--- a/code/processing/growth_curves_plate_reader/20210127_r1_MG1655_319_WT_UV5_tc/20210127_plate_layout.xlsx
+++ b/code/processing/growth_curves_plate_reader/20210127_r1_MG1655_319_WT_UV5_tc/20210127_plate_layout.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomroschinger/git/fit_seq/code/processing/growth_curves_plate_reader/20210127_r1_MG1655_WT_UV5_319_tc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomroschinger/git/fit_seq/code/processing/growth_curves_plate_reader/20210127_r1_MG1655_319_WT_UV5_tc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF97E4C3-6B9D-C647-9F0C-8BA1A9D7E15E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EACB2991-C859-4545-8312-1E1B9A8DBEA4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="strain" sheetId="1" r:id="rId1"/>
@@ -327,9 +327,6 @@
     <t>MG1655</t>
   </si>
   <si>
-    <t>blank</t>
-  </si>
-  <si>
     <t>3_19</t>
   </si>
   <si>
@@ -339,25 +336,28 @@
     <t>UV5</t>
   </si>
   <si>
-    <t>2.13_µg/ml_tc</t>
-  </si>
-  <si>
     <t>0_µg/ml_tc</t>
   </si>
   <si>
-    <t>4.57_µg/ml_tc</t>
-  </si>
-  <si>
-    <t>21.3_µg/ml_tc</t>
-  </si>
-  <si>
     <t>10_µg/ml_tc</t>
   </si>
   <si>
-    <t>45.7_µg/ml_tc</t>
-  </si>
-  <si>
     <t>100_µg/ml_tc</t>
+  </si>
+  <si>
+    <t>25_µg/ml_tc</t>
+  </si>
+  <si>
+    <t>40_µg/ml_tc</t>
+  </si>
+  <si>
+    <t>55_µg/ml_tc</t>
+  </si>
+  <si>
+    <t>70_µg/ml_tc</t>
+  </si>
+  <si>
+    <t>85_µg/ml_tc</t>
   </si>
 </sst>
 </file>
@@ -684,8 +684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -697,7 +697,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B1" t="s">
         <v>97</v>
@@ -706,31 +706,31 @@
         <v>97</v>
       </c>
       <c r="D1" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="E1" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="F1" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="G1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="H1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="I1" t="s">
-        <v>97</v>
-      </c>
-      <c r="J1" t="s">
-        <v>97</v>
-      </c>
-      <c r="K1" t="s">
-        <v>97</v>
-      </c>
-      <c r="L1" t="s">
-        <v>97</v>
+        <v>99</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -743,32 +743,32 @@
       <c r="C2" t="s">
         <v>97</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>99</v>
+      <c r="D2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F2" t="s">
+        <v>100</v>
       </c>
       <c r="G2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I2" t="s">
-        <v>100</v>
-      </c>
-      <c r="J2" t="s">
-        <v>101</v>
-      </c>
-      <c r="K2" t="s">
-        <v>101</v>
-      </c>
-      <c r="L2" t="s">
-        <v>101</v>
+        <v>99</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -781,32 +781,32 @@
       <c r="C3" t="s">
         <v>97</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>99</v>
+      <c r="D3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E3" t="s">
+        <v>100</v>
+      </c>
+      <c r="F3" t="s">
+        <v>100</v>
       </c>
       <c r="G3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I3" t="s">
-        <v>100</v>
-      </c>
-      <c r="J3" t="s">
-        <v>101</v>
-      </c>
-      <c r="K3" t="s">
-        <v>101</v>
-      </c>
-      <c r="L3" t="s">
-        <v>101</v>
+        <v>99</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -819,32 +819,32 @@
       <c r="C4" t="s">
         <v>97</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>99</v>
+      <c r="D4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E4" t="s">
+        <v>100</v>
+      </c>
+      <c r="F4" t="s">
+        <v>100</v>
       </c>
       <c r="G4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I4" t="s">
-        <v>100</v>
-      </c>
-      <c r="J4" t="s">
-        <v>101</v>
-      </c>
-      <c r="K4" t="s">
-        <v>101</v>
-      </c>
-      <c r="L4" t="s">
-        <v>101</v>
+        <v>99</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -857,32 +857,32 @@
       <c r="C5" t="s">
         <v>97</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>99</v>
+      <c r="D5" t="s">
+        <v>100</v>
+      </c>
+      <c r="E5" t="s">
+        <v>100</v>
+      </c>
+      <c r="F5" t="s">
+        <v>100</v>
       </c>
       <c r="G5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I5" t="s">
-        <v>100</v>
-      </c>
-      <c r="J5" t="s">
-        <v>101</v>
-      </c>
-      <c r="K5" t="s">
-        <v>101</v>
-      </c>
-      <c r="L5" t="s">
-        <v>101</v>
+        <v>99</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -895,32 +895,32 @@
       <c r="C6" t="s">
         <v>97</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>99</v>
+      <c r="D6" t="s">
+        <v>100</v>
+      </c>
+      <c r="E6" t="s">
+        <v>100</v>
+      </c>
+      <c r="F6" t="s">
+        <v>100</v>
       </c>
       <c r="G6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I6" t="s">
-        <v>100</v>
-      </c>
-      <c r="J6" t="s">
-        <v>101</v>
-      </c>
-      <c r="K6" t="s">
-        <v>101</v>
-      </c>
-      <c r="L6" t="s">
-        <v>101</v>
+        <v>99</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -933,32 +933,32 @@
       <c r="C7" t="s">
         <v>97</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>99</v>
+      <c r="D7" t="s">
+        <v>100</v>
+      </c>
+      <c r="E7" t="s">
+        <v>100</v>
+      </c>
+      <c r="F7" t="s">
+        <v>100</v>
       </c>
       <c r="G7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I7" t="s">
-        <v>100</v>
-      </c>
-      <c r="J7" t="s">
-        <v>101</v>
-      </c>
-      <c r="K7" t="s">
-        <v>101</v>
-      </c>
-      <c r="L7" t="s">
-        <v>101</v>
+        <v>99</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -971,32 +971,32 @@
       <c r="C8" t="s">
         <v>97</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>99</v>
+      <c r="D8" t="s">
+        <v>100</v>
+      </c>
+      <c r="E8" t="s">
+        <v>100</v>
+      </c>
+      <c r="F8" t="s">
+        <v>100</v>
       </c>
       <c r="G8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I8" t="s">
-        <v>100</v>
-      </c>
-      <c r="J8" t="s">
-        <v>101</v>
-      </c>
-      <c r="K8" t="s">
-        <v>101</v>
-      </c>
-      <c r="L8" t="s">
-        <v>101</v>
+        <v>99</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1650,8 +1650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1661,154 +1661,154 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="L2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B3" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C3" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D3" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E3" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="F3" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="G3" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="H3" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="I3" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="J3" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="K3" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="L3" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="G4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="I4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="J4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="K4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="L4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -1851,116 +1851,116 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B6" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C6" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D6" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E6" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="F6" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="G6" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="H6" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="I6" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="J6" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="K6" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="L6" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="G7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="I7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="J7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="K7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="L7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B8" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C8" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D8" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E8" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F8" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="G8" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="H8" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="I8" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="J8" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="K8" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="L8" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>